<commit_message>
KIBON-1292: Statistik mit "Zahlung ausgelöst" Funktion
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\kiBon\statistiken\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7C9112-4741-4DCA-BADC-119191FDF486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48674E4C-12B2-46EB-ADB6-7BBEE4EFB004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
   <si>
     <t>Typ</t>
   </si>
@@ -56,48 +56,12 @@
     <t>E-Mail</t>
   </si>
   <si>
-    <t>Tagesstätte für Kleinkinder</t>
-  </si>
-  <si>
-    <t>Verein kiPlus</t>
-  </si>
-  <si>
-    <t>Kita Tubehüsli</t>
-  </si>
-  <si>
-    <t>KiPlus Verein familienergänzende Kinderbetreuung Belp</t>
-  </si>
-  <si>
-    <t>Seftigenstrasse 85</t>
-  </si>
-  <si>
-    <t>3123</t>
-  </si>
-  <si>
-    <t>Belp</t>
-  </si>
-  <si>
-    <t>031 530 18 14</t>
-  </si>
-  <si>
-    <t>daniela.schmutz@kiplus.ch</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>PLZ</t>
   </si>
   <si>
     <t>Adresse</t>
   </si>
   <si>
-    <t>In Bearbeitung Institution - Stufe 2</t>
-  </si>
-  <si>
-    <t>Verfügt</t>
-  </si>
-  <si>
     <t>Kostenübernahme Anzahl Tage</t>
   </si>
   <si>
@@ -146,9 +110,6 @@
     <t>IBAN-Nummer</t>
   </si>
   <si>
-    <t>CH33 0900 0000 3000 0823 3</t>
-  </si>
-  <si>
     <t>Kontoinhaber</t>
   </si>
   <si>
@@ -162,9 +123,6 @@
   </si>
   <si>
     <t>Offene Zahlungen auslösen</t>
-  </si>
-  <si>
-    <t>Seftigenstrasse</t>
   </si>
   <si>
     <t>{datumErstellt}</t>
@@ -414,37 +372,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -452,6 +400,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -463,11 +414,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -782,11 +731,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B870EA-34FC-4BE3-9CEB-ADB0F6D1B0FC}">
-  <dimension ref="A1:AL9"/>
+  <dimension ref="A1:AL7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -808,104 +755,104 @@
   <sheetData>
     <row r="1" spans="1:38" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>44</v>
+        <v>28</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="15"/>
-      <c r="AB4" s="15"/>
-      <c r="AC4" s="16"/>
+        <v>29</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="13"/>
+      <c r="AC4" s="14"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE5" s="18"/>
-      <c r="AF5" s="18"/>
-      <c r="AG5" s="18"/>
-      <c r="AH5" s="18"/>
-      <c r="AI5" s="18"/>
-      <c r="AJ5" s="18"/>
-      <c r="AK5" s="19"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="17"/>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="17"/>
+      <c r="AI5" s="17"/>
+      <c r="AJ5" s="17"/>
+      <c r="AK5" s="18"/>
     </row>
     <row r="6" spans="1:38" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -917,16 +864,16 @@
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>4</v>
@@ -934,422 +881,214 @@
       <c r="K6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="V6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF6" s="7" t="s">
-        <v>38</v>
+      <c r="L6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF6" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="AG6" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="AH6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="AI6" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="AJ6" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="P7" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="R7" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="S7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="T7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="U7" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="V7" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="W7" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="X7" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y7" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L7" s="3" t="s">
+      <c r="Z7" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="AA7" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="AB7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="O7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="W7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="X7" s="3" t="s">
+      <c r="AC7" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="Y7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD7" s="8" t="e">
+      <c r="AD7" s="6" t="e">
         <f>AA7-R7</f>
         <v>#VALUE!</v>
       </c>
       <c r="AE7" s="3" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="AF7" s="3" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="AG7" s="3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="AH7" s="3" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="AI7" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="AJ7" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="AK7" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AL7" s="22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="3">
-        <v>85</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="3">
-        <v>0</v>
-      </c>
-      <c r="M8" s="3"/>
-      <c r="N8" s="6">
-        <v>5000</v>
-      </c>
-      <c r="O8" s="3">
-        <v>0</v>
-      </c>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="6">
-        <v>5000</v>
-      </c>
-      <c r="R8" s="8">
-        <f>O8*25+P8*1+Q8</f>
-        <v>5000</v>
-      </c>
-      <c r="S8" s="9">
-        <v>43952</v>
-      </c>
-      <c r="T8" s="11">
-        <v>43955</v>
-      </c>
-      <c r="U8" s="3">
-        <v>0</v>
-      </c>
-      <c r="V8" s="3"/>
-      <c r="W8" s="6">
-        <v>5000</v>
-      </c>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="8">
-        <f>X8*25+Y8*1+Z8</f>
-        <v>0</v>
-      </c>
-      <c r="AB8" s="5">
-        <v>26</v>
-      </c>
-      <c r="AC8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD8" s="8">
-        <f>R8</f>
-        <v>5000</v>
-      </c>
-      <c r="AE8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AH8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI8" s="3"/>
-      <c r="AJ8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK8" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="3">
-        <v>85</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="3">
-        <v>5</v>
-      </c>
-      <c r="M9" s="3"/>
-      <c r="N9" s="6">
-        <v>1000</v>
-      </c>
-      <c r="O9" s="3">
-        <v>6</v>
-      </c>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="6">
-        <v>1000</v>
-      </c>
-      <c r="R9" s="8">
-        <f>O9*25+P9*1+Q9</f>
-        <v>1150</v>
-      </c>
-      <c r="S9" s="9">
-        <v>43941</v>
-      </c>
-      <c r="T9" s="9">
-        <v>43946</v>
-      </c>
-      <c r="U9" s="3">
-        <v>6</v>
-      </c>
-      <c r="V9" s="3"/>
-      <c r="W9" s="6">
-        <v>1100</v>
-      </c>
-      <c r="X9" s="3">
-        <v>6</v>
-      </c>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="6">
-        <v>1100</v>
-      </c>
-      <c r="AA9" s="8">
-        <f>X9*25+Y9*1+Z9</f>
-        <v>1250</v>
-      </c>
-      <c r="AB9" s="5">
-        <v>26</v>
-      </c>
-      <c r="AC9" s="11">
-        <v>43955</v>
-      </c>
-      <c r="AD9" s="8">
-        <f>AA9-R9</f>
-        <v>100</v>
-      </c>
-      <c r="AE9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AH9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI9" s="3"/>
-      <c r="AJ9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK9" s="3" t="s">
-        <v>13</v>
+        <v>68</v>
+      </c>
+      <c r="AL7" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="R5:T5"/>
     <mergeCell ref="U4:AC4"/>
     <mergeCell ref="U5:W5"/>
     <mergeCell ref="X5:Z5"/>
     <mergeCell ref="AA5:AC5"/>
     <mergeCell ref="AD5:AK5"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="R5:T5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1357,9 +1096,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1560,27 +1302,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5629F10-0798-4A91-8A47-B660EE7C0BA9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A18E2A5-8E58-4041-8327-21E9E81899ED}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="55df0d9a-b115-40a4-96c1-9261dc1f94e8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d53bc33c-7e51-42d1-8a72-72bcbf7ea968"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1605,9 +1335,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A18E2A5-8E58-4041-8327-21E9E81899ED}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5629F10-0798-4A91-8A47-B660EE7C0BA9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="55df0d9a-b115-40a4-96c1-9261dc1f94e8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d53bc33c-7e51-42d1-8a72-72bcbf7ea968"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
KIBON-1307 Excel angepasst und Textänderungen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9641FBFD-B2B0-4F01-9E88-639902B1C203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683108D8-28D4-487C-A307-6B82F4C7BB96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t>Typ</t>
   </si>
@@ -62,12 +62,6 @@
     <t>Adresse</t>
   </si>
   <si>
-    <t>Kostenübernahme Anzahl Tage</t>
-  </si>
-  <si>
-    <t>Kostenübernahme Anzahl Stunden</t>
-  </si>
-  <si>
     <t>Kostenübrernahme Betreuung</t>
   </si>
   <si>
@@ -240,6 +234,21 @@
   </si>
   <si>
     <t>Zahlung freigegeben am</t>
+  </si>
+  <si>
+    <t>Rückerstattung Kanton für nicht angebotene Betreuungstage</t>
+  </si>
+  <si>
+    <t>Rückerstattung Kanton für nicht angebotene Betreuungsstunden</t>
+  </si>
+  <si>
+    <t>Zahlung ausgelöst</t>
+  </si>
+  <si>
+    <t>{stufe1ZahlungJetztAusgeloest}</t>
+  </si>
+  <si>
+    <t>{stufe2ZahlungJetztAusgeloest}</t>
   </si>
 </sst>
 </file>
@@ -372,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -416,6 +425,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -731,51 +743,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B870EA-34FC-4BE3-9CEB-ADB0F6D1B0FC}">
-  <dimension ref="A1:AL7"/>
+  <dimension ref="A1:AN7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" customWidth="1"/>
-    <col min="9" max="9" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="30" width="16.6640625" customWidth="1"/>
-    <col min="31" max="31" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="38" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="22.5703125" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+    <col min="15" max="16" width="23.42578125" customWidth="1"/>
+    <col min="17" max="21" width="16.7109375" customWidth="1"/>
+    <col min="22" max="23" width="22.7109375" customWidth="1"/>
+    <col min="24" max="24" width="16.7109375" customWidth="1"/>
+    <col min="25" max="26" width="22.85546875" customWidth="1"/>
+    <col min="27" max="32" width="16.7109375" customWidth="1"/>
+    <col min="33" max="33" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="40" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:40" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>30</v>
-      </c>
       <c r="L4" s="16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
@@ -784,20 +803,22 @@
       <c r="Q4" s="17"/>
       <c r="R4" s="17"/>
       <c r="S4" s="17"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="V4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="16" t="s">
+        <v>18</v>
+      </c>
       <c r="W4" s="17"/>
       <c r="X4" s="17"/>
       <c r="Y4" s="17"/>
       <c r="Z4" s="17"/>
       <c r="AA4" s="17"/>
       <c r="AB4" s="17"/>
-      <c r="AC4" s="18"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="18"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="F5" s="15" t="s">
         <v>8</v>
       </c>
@@ -807,52 +828,54 @@
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
       <c r="L5" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M5" s="15"/>
       <c r="N5" s="15"/>
       <c r="O5" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P5" s="15"/>
       <c r="Q5" s="15"/>
       <c r="R5" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="S5" s="15"/>
       <c r="T5" s="15"/>
-      <c r="U5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="V5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="W5" s="15"/>
-      <c r="X5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="Z5" s="15"/>
-      <c r="AA5" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="AC5" s="15"/>
-      <c r="AD5" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE5" s="20"/>
-      <c r="AF5" s="20"/>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="19" t="s">
+        <v>20</v>
+      </c>
       <c r="AG5" s="20"/>
       <c r="AH5" s="20"/>
       <c r="AI5" s="20"/>
       <c r="AJ5" s="20"/>
-      <c r="AK5" s="21"/>
+      <c r="AK5" s="20"/>
+      <c r="AL5" s="20"/>
+      <c r="AM5" s="21"/>
     </row>
-    <row r="6" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -864,13 +887,13 @@
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>7</v>
@@ -882,235 +905,238 @@
         <v>5</v>
       </c>
       <c r="L6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="N6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="O6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q6" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="R6" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="T6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="W6" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="U6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W6" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="X6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="Z6" s="5" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="AB6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="AE6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AF6" s="5" t="s">
+      <c r="AJ6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AG6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ6" s="2" t="s">
+      <c r="AL6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AK6" s="2" t="s">
+      <c r="AM6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="D7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="E7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="L7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="N7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="U7" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="V7" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="W7" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z7" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE7" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF7" s="6" t="str">
+        <f>IF(AE7="Ja",AB7-R7,IF(U7="Ja",R7,"-"))</f>
+        <v>-</v>
+      </c>
+      <c r="AG7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="AJ7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="P7" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q7" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="R7" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="U7" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="V7" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="W7" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="X7" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y7" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z7" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA7" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB7" s="4" t="s">
+      <c r="AK7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN7" s="10" t="s">
         <v>53</v>
-      </c>
-      <c r="AC7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD7" s="6" t="str">
-        <f ca="1">IF(AND(T7=TODAY(),AC7&lt;&gt;TODAY()),R7,IF(AC7=TODAY(),AA7-R7,""))</f>
-        <v/>
-      </c>
-      <c r="AE7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AJ7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AL7" s="10" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="U4:AC4"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="X5:Z5"/>
-    <mergeCell ref="AA5:AC5"/>
-    <mergeCell ref="AD5:AK5"/>
+    <mergeCell ref="V4:AE4"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="AB5:AE5"/>
+    <mergeCell ref="AF5:AM5"/>
     <mergeCell ref="F5:K5"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="L4:U4"/>
+    <mergeCell ref="R5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100711209C60F5007419C092DB1F82A4795" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ddb10cc1903f988a2bdc77454b9dc4c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d53bc33c-7e51-42d1-8a72-72bcbf7ea968" xmlns:ns3="55df0d9a-b115-40a4-96c1-9261dc1f94e8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c657c3bfd70ec264372646d204a4f2b" ns2:_="" ns3:_="">
     <xsd:import namespace="d53bc33c-7e51-42d1-8a72-72bcbf7ea968"/>
@@ -1307,15 +1333,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A18E2A5-8E58-4041-8327-21E9E81899ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5629F10-0798-4A91-8A47-B660EE7C0BA9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1332,7 +1359,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA59B390-4D54-40A4-8874-4D75877374A7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1349,4 +1376,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A18E2A5-8E58-4041-8327-21E9E81899ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
KIBON-1485: Notverordnung: Spalte privat/öffentlich zu Excel hinzufügen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Transfer\kiBon-Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683108D8-28D4-487C-A307-6B82F4C7BB96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE6466B-6A41-4D9D-85F5-8F997C92E908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
+    <workbookView xWindow="-25800" yWindow="2715" windowWidth="21600" windowHeight="11385" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
   <si>
     <t>Typ</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>{stufe2ZahlungJetztAusgeloest}</t>
+  </si>
+  <si>
+    <t>Privat oder öffentlich</t>
+  </si>
+  <si>
+    <t>{institutionTyp}</t>
   </si>
 </sst>
 </file>
@@ -381,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -408,6 +414,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -415,6 +427,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -426,8 +441,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,7 +758,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B870EA-34FC-4BE3-9CEB-ADB0F6D1B0FC}">
-  <dimension ref="A1:AN7"/>
+  <dimension ref="A1:AO7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -763,22 +778,22 @@
     <col min="12" max="13" width="22.5703125" customWidth="1"/>
     <col min="14" max="14" width="16.7109375" customWidth="1"/>
     <col min="15" max="16" width="23.42578125" customWidth="1"/>
-    <col min="17" max="21" width="16.7109375" customWidth="1"/>
-    <col min="22" max="23" width="22.7109375" customWidth="1"/>
-    <col min="24" max="24" width="16.7109375" customWidth="1"/>
-    <col min="25" max="26" width="22.85546875" customWidth="1"/>
-    <col min="27" max="32" width="16.7109375" customWidth="1"/>
-    <col min="33" max="33" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="40" width="16.7109375" customWidth="1"/>
+    <col min="17" max="22" width="16.7109375" customWidth="1"/>
+    <col min="23" max="24" width="22.7109375" customWidth="1"/>
+    <col min="25" max="25" width="16.7109375" customWidth="1"/>
+    <col min="26" max="27" width="22.85546875" customWidth="1"/>
+    <col min="28" max="33" width="16.7109375" customWidth="1"/>
+    <col min="34" max="34" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="41" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
@@ -786,91 +801,93 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="16" t="s">
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="W4" s="17"/>
-      <c r="X4" s="17"/>
-      <c r="Y4" s="17"/>
-      <c r="Z4" s="17"/>
-      <c r="AA4" s="17"/>
-      <c r="AB4" s="17"/>
-      <c r="AC4" s="17"/>
-      <c r="AD4" s="17"/>
-      <c r="AE4" s="18"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="19"/>
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="20"/>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="F5" s="15" t="s">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="F5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15" t="s">
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15" t="s">
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15" t="s">
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15" t="s">
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15" t="s">
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15" t="s">
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="21"/>
+      <c r="AC5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="19" t="s">
+      <c r="AD5" s="21"/>
+      <c r="AE5" s="21"/>
+      <c r="AF5" s="21"/>
+      <c r="AG5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="AG5" s="20"/>
-      <c r="AH5" s="20"/>
-      <c r="AI5" s="20"/>
-      <c r="AJ5" s="20"/>
-      <c r="AK5" s="20"/>
-      <c r="AL5" s="20"/>
-      <c r="AM5" s="21"/>
+      <c r="AH5" s="23"/>
+      <c r="AI5" s="23"/>
+      <c r="AJ5" s="23"/>
+      <c r="AK5" s="23"/>
+      <c r="AL5" s="23"/>
+      <c r="AM5" s="23"/>
+      <c r="AN5" s="24"/>
     </row>
-    <row r="6" spans="1:40" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -935,61 +952,64 @@
         <v>69</v>
       </c>
       <c r="V6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="W6" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="W6" s="5" t="s">
+      <c r="X6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="X6" s="5" t="s">
+      <c r="Y6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Y6" s="5" t="s">
+      <c r="Z6" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="Z6" s="5" t="s">
+      <c r="AA6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AA6" s="5" t="s">
+      <c r="AB6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AB6" s="5" t="s">
+      <c r="AC6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AC6" s="5" t="s">
+      <c r="AD6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AD6" s="5" t="s">
+      <c r="AE6" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="AE6" s="5" t="s">
+      <c r="AF6" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AF6" s="5" t="s">
+      <c r="AG6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AG6" s="5" t="s">
+      <c r="AH6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AH6" s="5" t="s">
+      <c r="AI6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AI6" s="2" t="s">
+      <c r="AJ6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AJ6" s="2" t="s">
+      <c r="AK6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AK6" s="2" t="s">
+      <c r="AL6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AL6" s="2" t="s">
+      <c r="AM6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AM6" s="2" t="s">
+      <c r="AN6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>29</v>
       </c>
@@ -1050,80 +1070,83 @@
       <c r="T7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="U7" s="22" t="s">
+      <c r="U7" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="V7" s="13" t="s">
+      <c r="V7" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="W7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="W7" s="13" t="s">
+      <c r="X7" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="X7" s="12" t="s">
+      <c r="Y7" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="Y7" s="13" t="s">
+      <c r="Z7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="Z7" s="13" t="s">
+      <c r="AA7" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="AA7" s="12" t="s">
+      <c r="AB7" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AB7" s="12" t="s">
+      <c r="AC7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="AC7" s="4" t="s">
+      <c r="AD7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AD7" s="4" t="s">
+      <c r="AE7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AE7" s="22" t="s">
+      <c r="AF7" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="AF7" s="6" t="str">
-        <f>IF(AE7="Ja",AB7-R7,IF(U7="Ja",R7,"-"))</f>
+      <c r="AG7" s="6" t="str">
+        <f>IF(AF7="Ja",AC7-R7,IF(U7="Ja",R7,"-"))</f>
         <v>-</v>
       </c>
-      <c r="AG7" s="3" t="s">
+      <c r="AH7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AH7" s="3" t="s">
+      <c r="AI7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AI7" s="3" t="s">
+      <c r="AJ7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="AJ7" s="3" t="s">
+      <c r="AK7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AK7" s="3" t="s">
+      <c r="AL7" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AL7" s="3" t="s">
+      <c r="AM7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AM7" s="3" t="s">
+      <c r="AN7" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AN7" s="10" t="s">
+      <c r="AO7" s="10" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="V4:AE4"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="AB5:AE5"/>
-    <mergeCell ref="AF5:AM5"/>
     <mergeCell ref="F5:K5"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="L4:U4"/>
     <mergeCell ref="R5:U5"/>
+    <mergeCell ref="W4:AF4"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="Z5:AB5"/>
+    <mergeCell ref="AC5:AF5"/>
+    <mergeCell ref="AG5:AN5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1137,6 +1160,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100711209C60F5007419C092DB1F82A4795" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ddb10cc1903f988a2bdc77454b9dc4c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d53bc33c-7e51-42d1-8a72-72bcbf7ea968" xmlns:ns3="55df0d9a-b115-40a4-96c1-9261dc1f94e8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c657c3bfd70ec264372646d204a4f2b" ns2:_="" ns3:_="">
     <xsd:import namespace="d53bc33c-7e51-42d1-8a72-72bcbf7ea968"/>
@@ -1333,15 +1365,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5629F10-0798-4A91-8A47-B660EE7C0BA9}">
   <ds:schemaRefs>
@@ -1360,6 +1383,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A18E2A5-8E58-4041-8327-21E9E81899ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA59B390-4D54-40A4-8874-4D75877374A7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1376,12 +1407,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A18E2A5-8E58-4041-8327-21E9E81899ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
KIBON-1416: Rückforderung: Excel Vorlage Anpassungen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Transfer\kiBon-Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE6466B-6A41-4D9D-85F5-8F997C92E908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DD7618-19D3-4F59-B753-A01D3516AF35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25800" yWindow="2715" windowWidth="21600" windowHeight="11385" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
+    <workbookView xWindow="6060" yWindow="1335" windowWidth="21600" windowHeight="11385" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
   <si>
     <t>Typ</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Betrag</t>
   </si>
   <si>
-    <t>Stufe 2</t>
-  </si>
-  <si>
     <t>Verfügung</t>
   </si>
   <si>
@@ -255,6 +252,42 @@
   </si>
   <si>
     <t>{institutionTyp}</t>
+  </si>
+  <si>
+    <t>Stufe 2 öffentlich</t>
+  </si>
+  <si>
+    <t>Stufe 2 privat</t>
+  </si>
+  <si>
+    <t>Betrag entgangene Elternbeiträge</t>
+  </si>
+  <si>
+    <t>Davon für nicht angebotene Tage oder Stunde</t>
+  </si>
+  <si>
+    <t>ausbezahlte Kurzarbeits- entschädigung</t>
+  </si>
+  <si>
+    <t>ausbezahlte Corona-Erwerbsersatz- entschädigung</t>
+  </si>
+  <si>
+    <t>Rückerstattung für nicht angebotene Betreuungstage gemäss kantonaler Notverordnung</t>
+  </si>
+  <si>
+    <t>{betragEntgangeneElternbeitraege}</t>
+  </si>
+  <si>
+    <t>{betragEntgangeneElternbeitraegeNichtAngeboteneEinheiten}</t>
+  </si>
+  <si>
+    <t>{rueckerstattungNichtAngeboteneBetreuungstage}</t>
+  </si>
+  <si>
+    <t>{kurzarbeitBetrag}</t>
+  </si>
+  <si>
+    <t>{coronaErwerbsersatzBetrag}</t>
   </si>
 </sst>
 </file>
@@ -301,7 +334,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -383,11 +416,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -420,6 +466,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -429,9 +481,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -441,8 +490,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,7 +812,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B870EA-34FC-4BE3-9CEB-ADB0F6D1B0FC}">
-  <dimension ref="A1:AO7"/>
+  <dimension ref="A1:AT7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -782,112 +836,134 @@
     <col min="23" max="24" width="22.7109375" customWidth="1"/>
     <col min="25" max="25" width="16.7109375" customWidth="1"/>
     <col min="26" max="27" width="22.85546875" customWidth="1"/>
-    <col min="28" max="33" width="16.7109375" customWidth="1"/>
-    <col min="34" max="34" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="41" width="16.7109375" customWidth="1"/>
+    <col min="28" max="38" width="16.7109375" customWidth="1"/>
+    <col min="39" max="39" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="46" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:46" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B4" s="14" t="s">
         <v>27</v>
       </c>
+      <c r="L4" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="21"/>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD4" s="21"/>
+      <c r="AE4" s="21"/>
+      <c r="AF4" s="21"/>
+      <c r="AG4" s="22"/>
+      <c r="AH4" s="26"/>
+      <c r="AI4" s="26"/>
+      <c r="AJ4" s="26"/>
+      <c r="AK4" s="27"/>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="18" t="s">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="F5" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD5" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE5" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF5" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG5" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19"/>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="19"/>
-      <c r="AE4" s="19"/>
-      <c r="AF4" s="20"/>
+      <c r="AI5" s="19"/>
+      <c r="AJ5" s="19"/>
+      <c r="AK5" s="19"/>
+      <c r="AL5" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM5" s="24"/>
+      <c r="AN5" s="24"/>
+      <c r="AO5" s="24"/>
+      <c r="AP5" s="24"/>
+      <c r="AQ5" s="24"/>
+      <c r="AR5" s="24"/>
+      <c r="AS5" s="25"/>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="F5" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="21"/>
-      <c r="AC5" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD5" s="21"/>
-      <c r="AE5" s="21"/>
-      <c r="AF5" s="21"/>
-      <c r="AG5" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="AH5" s="23"/>
-      <c r="AI5" s="23"/>
-      <c r="AJ5" s="23"/>
-      <c r="AK5" s="23"/>
-      <c r="AL5" s="23"/>
-      <c r="AM5" s="23"/>
-      <c r="AN5" s="24"/>
-    </row>
-    <row r="6" spans="1:41" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -904,13 +980,13 @@
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>7</v>
@@ -922,19 +998,19 @@
         <v>5</v>
       </c>
       <c r="L6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="N6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="O6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="P6" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="Q6" s="5" t="s">
         <v>9</v>
@@ -946,207 +1022,233 @@
         <v>15</v>
       </c>
       <c r="T6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="W6" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="U6" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="V6" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="W6" s="5" t="s">
+      <c r="X6" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="X6" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="Y6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="Z6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA6" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="AA6" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="AB6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AC6" s="5" t="s">
+      <c r="AC6" s="29"/>
+      <c r="AD6" s="29"/>
+      <c r="AE6" s="29"/>
+      <c r="AF6" s="29"/>
+      <c r="AG6" s="29"/>
+      <c r="AH6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AD6" s="5" t="s">
+      <c r="AI6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AE6" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF6" s="5" t="s">
+      <c r="AJ6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AO6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AS6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="U7" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="AG6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AH6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AJ6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AM6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AN6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="V7" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="W7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="X7" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA7" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD7" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE7" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF7" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG7" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK7" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL7" s="6" t="str">
+        <f>IF(AK7="Ja",AH7-R7,IF(U7="Ja",R7,"-"))</f>
+        <v>-</v>
+      </c>
+      <c r="AM7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="P7" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="R7" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="U7" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="V7" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="W7" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="X7" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y7" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z7" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA7" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB7" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC7" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE7" s="4" t="s">
+      <c r="AP7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT7" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="AF7" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG7" s="6" t="str">
-        <f>IF(AF7="Ja",AC7-R7,IF(U7="Ja",R7,"-"))</f>
-        <v>-</v>
-      </c>
-      <c r="AH7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AN7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AO7" s="10" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="16">
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="Z5:AB5"/>
+    <mergeCell ref="AH5:AK5"/>
+    <mergeCell ref="AL5:AS5"/>
+    <mergeCell ref="AC4:AG4"/>
+    <mergeCell ref="W4:AB4"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="AD5:AD6"/>
+    <mergeCell ref="AE5:AE6"/>
+    <mergeCell ref="AF5:AF6"/>
+    <mergeCell ref="AG5:AG6"/>
     <mergeCell ref="F5:K5"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="L4:U4"/>
     <mergeCell ref="R5:U5"/>
-    <mergeCell ref="W4:AF4"/>
-    <mergeCell ref="W5:Y5"/>
-    <mergeCell ref="Z5:AB5"/>
-    <mergeCell ref="AC5:AF5"/>
-    <mergeCell ref="AG5:AN5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1160,15 +1262,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100711209C60F5007419C092DB1F82A4795" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ddb10cc1903f988a2bdc77454b9dc4c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d53bc33c-7e51-42d1-8a72-72bcbf7ea968" xmlns:ns3="55df0d9a-b115-40a4-96c1-9261dc1f94e8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c657c3bfd70ec264372646d204a4f2b" ns2:_="" ns3:_="">
     <xsd:import namespace="d53bc33c-7e51-42d1-8a72-72bcbf7ea968"/>
@@ -1365,6 +1458,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5629F10-0798-4A91-8A47-B660EE7C0BA9}">
   <ds:schemaRefs>
@@ -1383,14 +1485,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A18E2A5-8E58-4041-8327-21E9E81899ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA59B390-4D54-40A4-8874-4D75877374A7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1407,4 +1501,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A18E2A5-8E58-4041-8327-21E9E81899ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
KIBON-1654 Beschwerde in Excel Zahlungen angepasst
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Transfer\kiBon-Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DD7618-19D3-4F59-B753-A01D3516AF35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F06894-F857-43BD-B59B-E0DEAF020D4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="1335" windowWidth="21600" windowHeight="11385" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
   <si>
     <t>Typ</t>
   </si>
@@ -288,6 +288,18 @@
   </si>
   <si>
     <t>{coronaErwerbsersatzBetrag}</t>
+  </si>
+  <si>
+    <t>Beschwerde</t>
+  </si>
+  <si>
+    <t>{beschwerdeBetrag}</t>
+  </si>
+  <si>
+    <t>{beschwerdeAusbezahltAm}</t>
+  </si>
+  <si>
+    <t>{beschwerdeZahlungJetztAusgeloest}</t>
   </si>
 </sst>
 </file>
@@ -334,7 +346,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -429,11 +441,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -481,22 +555,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -812,7 +899,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B870EA-34FC-4BE3-9CEB-ADB0F6D1B0FC}">
-  <dimension ref="A1:AT7"/>
+  <dimension ref="A1:AW7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -836,18 +923,18 @@
     <col min="23" max="24" width="22.7109375" customWidth="1"/>
     <col min="25" max="25" width="16.7109375" customWidth="1"/>
     <col min="26" max="27" width="22.85546875" customWidth="1"/>
-    <col min="28" max="38" width="16.7109375" customWidth="1"/>
-    <col min="39" max="39" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="46" width="16.7109375" customWidth="1"/>
+    <col min="28" max="41" width="16.7109375" customWidth="1"/>
+    <col min="42" max="42" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="49" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:49" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -855,7 +942,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
@@ -890,12 +977,19 @@
       <c r="AE4" s="21"/>
       <c r="AF4" s="21"/>
       <c r="AG4" s="22"/>
-      <c r="AH4" s="26"/>
-      <c r="AI4" s="26"/>
-      <c r="AJ4" s="26"/>
-      <c r="AK4" s="27"/>
+      <c r="AH4" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI4" s="28"/>
+      <c r="AJ4" s="28"/>
+      <c r="AK4" s="29"/>
+      <c r="AL4" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM4" s="28"/>
+      <c r="AN4" s="29"/>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="F5" s="19" t="s">
         <v>8</v>
       </c>
@@ -931,39 +1025,40 @@
       </c>
       <c r="AA5" s="19"/>
       <c r="AB5" s="19"/>
-      <c r="AC5" s="28" t="s">
+      <c r="AC5" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="AD5" s="28" t="s">
+      <c r="AD5" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="AE5" s="28" t="s">
+      <c r="AE5" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="AF5" s="28" t="s">
+      <c r="AF5" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="AG5" s="28" t="s">
+      <c r="AG5" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="AH5" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI5" s="19"/>
-      <c r="AJ5" s="19"/>
-      <c r="AK5" s="19"/>
-      <c r="AL5" s="23" t="s">
+      <c r="AH5" s="30"/>
+      <c r="AI5" s="31"/>
+      <c r="AJ5" s="31"/>
+      <c r="AK5" s="32"/>
+      <c r="AL5" s="30"/>
+      <c r="AM5" s="31"/>
+      <c r="AN5" s="32"/>
+      <c r="AO5" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="AM5" s="24"/>
-      <c r="AN5" s="24"/>
-      <c r="AO5" s="24"/>
-      <c r="AP5" s="24"/>
-      <c r="AQ5" s="24"/>
-      <c r="AR5" s="24"/>
-      <c r="AS5" s="25"/>
+      <c r="AP5" s="23"/>
+      <c r="AQ5" s="23"/>
+      <c r="AR5" s="23"/>
+      <c r="AS5" s="23"/>
+      <c r="AT5" s="23"/>
+      <c r="AU5" s="23"/>
+      <c r="AV5" s="24"/>
     </row>
-    <row r="6" spans="1:46" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1048,11 +1143,11 @@
       <c r="AB6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AC6" s="29"/>
-      <c r="AD6" s="29"/>
-      <c r="AE6" s="29"/>
-      <c r="AF6" s="29"/>
-      <c r="AG6" s="29"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="26"/>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="26"/>
+      <c r="AG6" s="26"/>
       <c r="AH6" s="5" t="s">
         <v>17</v>
       </c>
@@ -1069,28 +1164,37 @@
         <v>17</v>
       </c>
       <c r="AM6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AP6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="AN6" s="5" t="s">
+      <c r="AQ6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AO6" s="2" t="s">
+      <c r="AR6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AP6" s="2" t="s">
+      <c r="AS6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AQ6" s="2" t="s">
+      <c r="AT6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AR6" s="2" t="s">
+      <c r="AU6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AS6" s="2" t="s">
+      <c r="AV6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>28</v>
       </c>
@@ -1202,41 +1306,49 @@
       <c r="AK7" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="AL7" s="6" t="str">
-        <f>IF(AK7="Ja",AH7-R7,IF(U7="Ja",R7,"-"))</f>
+      <c r="AL7" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN7" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO7" s="6" t="str">
+        <f>IF(AN7="Ja",IF(AK7="Ja",AH7+AL7,AL7),IF(AK7="Ja",AH7-R7,IF(U7="Ja",R7,"-")))</f>
         <v>-</v>
       </c>
-      <c r="AM7" s="3" t="s">
+      <c r="AP7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AN7" s="3" t="s">
+      <c r="AQ7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AO7" s="3" t="s">
+      <c r="AR7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AP7" s="3" t="s">
+      <c r="AS7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="AQ7" s="3" t="s">
+      <c r="AT7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AR7" s="3" t="s">
+      <c r="AU7" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AS7" s="3" t="s">
+      <c r="AV7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AT7" s="10" t="s">
+      <c r="AW7" s="10" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
     <mergeCell ref="W5:Y5"/>
     <mergeCell ref="Z5:AB5"/>
-    <mergeCell ref="AH5:AK5"/>
-    <mergeCell ref="AL5:AS5"/>
+    <mergeCell ref="AO5:AV5"/>
     <mergeCell ref="AC4:AG4"/>
     <mergeCell ref="W4:AB4"/>
     <mergeCell ref="AC5:AC6"/>
@@ -1244,6 +1356,8 @@
     <mergeCell ref="AE5:AE6"/>
     <mergeCell ref="AF5:AF6"/>
     <mergeCell ref="AG5:AG6"/>
+    <mergeCell ref="AH4:AK5"/>
+    <mergeCell ref="AL4:AN5"/>
     <mergeCell ref="F5:K5"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="O5:Q5"/>

</xml_diff>

<commit_message>
KIBON-1654 Notrecht Excel angepasst
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F06894-F857-43BD-B59B-E0DEAF020D4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CF6207-78DF-490E-8B1E-98BCCC334BA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="91">
   <si>
     <t>Typ</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>{beschwerdeZahlungJetztAusgeloest}</t>
+  </si>
+  <si>
+    <t>Definitiver Verfügungsbetrag</t>
+  </si>
+  <si>
+    <t>Betrag Auszahlung</t>
   </si>
 </sst>
 </file>
@@ -346,7 +352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -503,11 +509,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -546,6 +563,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -555,12 +578,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -584,6 +601,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,7 +928,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B870EA-34FC-4BE3-9CEB-ADB0F6D1B0FC}">
-  <dimension ref="A1:AW7"/>
+  <dimension ref="A1:AX7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -923,18 +952,18 @@
     <col min="23" max="24" width="22.7109375" customWidth="1"/>
     <col min="25" max="25" width="16.7109375" customWidth="1"/>
     <col min="26" max="27" width="22.85546875" customWidth="1"/>
-    <col min="28" max="41" width="16.7109375" customWidth="1"/>
-    <col min="42" max="42" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="49" width="16.7109375" customWidth="1"/>
+    <col min="28" max="42" width="16.7109375" customWidth="1"/>
+    <col min="43" max="43" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="50" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:50" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -942,41 +971,41 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="22"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="24"/>
       <c r="V4" s="16"/>
-      <c r="W4" s="20" t="s">
+      <c r="W4" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="21"/>
-      <c r="Z4" s="21"/>
-      <c r="AA4" s="21"/>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="20" t="s">
+      <c r="X4" s="23"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="AD4" s="21"/>
-      <c r="AE4" s="21"/>
-      <c r="AF4" s="21"/>
-      <c r="AG4" s="22"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="24"/>
       <c r="AH4" s="27" t="s">
         <v>18</v>
       </c>
@@ -988,8 +1017,11 @@
       </c>
       <c r="AM4" s="28"/>
       <c r="AN4" s="29"/>
+      <c r="AO4" s="34" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="F5" s="19" t="s">
         <v>8</v>
       </c>
@@ -1047,18 +1079,19 @@
       <c r="AL5" s="30"/>
       <c r="AM5" s="31"/>
       <c r="AN5" s="32"/>
-      <c r="AO5" s="23" t="s">
+      <c r="AO5" s="35"/>
+      <c r="AP5" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="AP5" s="23"/>
-      <c r="AQ5" s="23"/>
-      <c r="AR5" s="23"/>
-      <c r="AS5" s="23"/>
-      <c r="AT5" s="23"/>
-      <c r="AU5" s="23"/>
-      <c r="AV5" s="24"/>
+      <c r="AQ5" s="20"/>
+      <c r="AR5" s="20"/>
+      <c r="AS5" s="20"/>
+      <c r="AT5" s="20"/>
+      <c r="AU5" s="20"/>
+      <c r="AV5" s="20"/>
+      <c r="AW5" s="21"/>
     </row>
-    <row r="6" spans="1:49" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1169,32 +1202,33 @@
       <c r="AN6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AO6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AP6" s="5" t="s">
+      <c r="AO6" s="36"/>
+      <c r="AP6" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="AQ6" s="5" t="s">
+      <c r="AR6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AR6" s="2" t="s">
+      <c r="AS6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AS6" s="2" t="s">
+      <c r="AT6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AT6" s="2" t="s">
+      <c r="AU6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AU6" s="2" t="s">
+      <c r="AV6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AV6" s="2" t="s">
+      <c r="AW6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>28</v>
       </c>
@@ -1315,40 +1349,49 @@
       <c r="AN7" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="AO7" s="6" t="str">
-        <f>IF(AN7="Ja",IF(AK7="Ja",AH7+AL7,AL7),IF(AK7="Ja",AH7-R7,IF(U7="Ja",R7,"-")))</f>
+      <c r="AO7" s="17" t="str">
+        <f>IF(NOT(ISNUMBER(AL7)),AL7,AH7)</f>
+        <v>{beschwerdeBetrag}</v>
+      </c>
+      <c r="AP7" s="6" t="str">
+        <f>IF(AN7="Ja",IF(AK7="Ja",AL7,AL7-AH7),IF(AK7="Ja",AH7-R7,IF(U7="Ja",R7,"-")))</f>
         <v>-</v>
       </c>
-      <c r="AP7" s="3" t="s">
+      <c r="AQ7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AQ7" s="3" t="s">
+      <c r="AR7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AR7" s="3" t="s">
+      <c r="AS7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AS7" s="3" t="s">
+      <c r="AT7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="AT7" s="3" t="s">
+      <c r="AU7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AU7" s="3" t="s">
+      <c r="AV7" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AV7" s="3" t="s">
+      <c r="AW7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AW7" s="10" t="s">
+      <c r="AX7" s="10" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="L4:U4"/>
+    <mergeCell ref="R5:U5"/>
     <mergeCell ref="W5:Y5"/>
     <mergeCell ref="Z5:AB5"/>
-    <mergeCell ref="AO5:AV5"/>
+    <mergeCell ref="AP5:AW5"/>
     <mergeCell ref="AC4:AG4"/>
     <mergeCell ref="W4:AB4"/>
     <mergeCell ref="AC5:AC6"/>
@@ -1358,11 +1401,7 @@
     <mergeCell ref="AG5:AG6"/>
     <mergeCell ref="AH4:AK5"/>
     <mergeCell ref="AL4:AN5"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="L4:U4"/>
-    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="AO4:AO6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1370,12 +1409,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100711209C60F5007419C092DB1F82A4795" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ddb10cc1903f988a2bdc77454b9dc4c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d53bc33c-7e51-42d1-8a72-72bcbf7ea968" xmlns:ns3="55df0d9a-b115-40a4-96c1-9261dc1f94e8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c657c3bfd70ec264372646d204a4f2b" ns2:_="" ns3:_="">
     <xsd:import namespace="d53bc33c-7e51-42d1-8a72-72bcbf7ea968"/>
@@ -1572,6 +1605,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1582,23 +1621,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5629F10-0798-4A91-8A47-B660EE7C0BA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="55df0d9a-b115-40a4-96c1-9261dc1f94e8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d53bc33c-7e51-42d1-8a72-72bcbf7ea968"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA59B390-4D54-40A4-8874-4D75877374A7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1617,6 +1639,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5629F10-0798-4A91-8A47-B660EE7C0BA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="55df0d9a-b115-40a4-96c1-9261dc1f94e8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d53bc33c-7e51-42d1-8a72-72bcbf7ea968"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A18E2A5-8E58-4041-8327-21E9E81899ED}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
direct-to-dev: Formel in Notrecht Excel Template angepasst
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CF6207-78DF-490E-8B1E-98BCCC334BA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B449DFFE-A155-4F4C-B4D0-AFB9113496EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -560,24 +560,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -601,9 +604,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -978,118 +978,118 @@
       <c r="B4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="22" t="s">
+      <c r="L4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="24"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="23"/>
       <c r="V4" s="16"/>
-      <c r="W4" s="22" t="s">
+      <c r="W4" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="23"/>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="22" t="s">
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="AD4" s="23"/>
-      <c r="AE4" s="23"/>
-      <c r="AF4" s="23"/>
-      <c r="AG4" s="24"/>
-      <c r="AH4" s="27" t="s">
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="23"/>
+      <c r="AH4" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="AI4" s="28"/>
-      <c r="AJ4" s="28"/>
-      <c r="AK4" s="29"/>
-      <c r="AL4" s="27" t="s">
+      <c r="AI4" s="29"/>
+      <c r="AJ4" s="29"/>
+      <c r="AK4" s="30"/>
+      <c r="AL4" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="AM4" s="28"/>
-      <c r="AN4" s="29"/>
+      <c r="AM4" s="29"/>
+      <c r="AN4" s="30"/>
       <c r="AO4" s="34" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19" t="s">
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19" t="s">
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19" t="s">
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
       <c r="V5" s="15"/>
-      <c r="W5" s="19" t="s">
+      <c r="W5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="19"/>
-      <c r="Z5" s="19" t="s">
+      <c r="X5" s="20"/>
+      <c r="Y5" s="20"/>
+      <c r="Z5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
-      <c r="AC5" s="25" t="s">
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="AD5" s="25" t="s">
+      <c r="AD5" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="AE5" s="25" t="s">
+      <c r="AE5" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="AF5" s="25" t="s">
+      <c r="AF5" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="AG5" s="25" t="s">
+      <c r="AG5" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="AH5" s="30"/>
-      <c r="AI5" s="31"/>
-      <c r="AJ5" s="31"/>
-      <c r="AK5" s="32"/>
-      <c r="AL5" s="30"/>
-      <c r="AM5" s="31"/>
-      <c r="AN5" s="32"/>
+      <c r="AH5" s="31"/>
+      <c r="AI5" s="32"/>
+      <c r="AJ5" s="32"/>
+      <c r="AK5" s="33"/>
+      <c r="AL5" s="31"/>
+      <c r="AM5" s="32"/>
+      <c r="AN5" s="33"/>
       <c r="AO5" s="35"/>
-      <c r="AP5" s="20" t="s">
+      <c r="AP5" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="AQ5" s="20"/>
-      <c r="AR5" s="20"/>
-      <c r="AS5" s="20"/>
-      <c r="AT5" s="20"/>
-      <c r="AU5" s="20"/>
-      <c r="AV5" s="20"/>
-      <c r="AW5" s="21"/>
+      <c r="AQ5" s="24"/>
+      <c r="AR5" s="24"/>
+      <c r="AS5" s="24"/>
+      <c r="AT5" s="24"/>
+      <c r="AU5" s="24"/>
+      <c r="AV5" s="24"/>
+      <c r="AW5" s="25"/>
     </row>
     <row r="6" spans="1:50" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1176,11 +1176,11 @@
       <c r="AB6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AC6" s="26"/>
-      <c r="AD6" s="26"/>
-      <c r="AE6" s="26"/>
-      <c r="AF6" s="26"/>
-      <c r="AG6" s="26"/>
+      <c r="AC6" s="27"/>
+      <c r="AD6" s="27"/>
+      <c r="AE6" s="27"/>
+      <c r="AF6" s="27"/>
+      <c r="AG6" s="27"/>
       <c r="AH6" s="5" t="s">
         <v>17</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>68</v>
       </c>
       <c r="AO6" s="36"/>
-      <c r="AP6" s="33" t="s">
+      <c r="AP6" s="19" t="s">
         <v>90</v>
       </c>
       <c r="AQ6" s="5" t="s">
@@ -1350,8 +1350,8 @@
         <v>88</v>
       </c>
       <c r="AO7" s="17" t="str">
-        <f>IF(NOT(ISNUMBER(AL7)),AL7,AH7)</f>
-        <v>{beschwerdeBetrag}</v>
+        <f>IF(NOT(ISNUMBER(AL7)),AH7,AL7)</f>
+        <v>{stufe2VerfuegungBetrag}</v>
       </c>
       <c r="AP7" s="6" t="str">
         <f>IF(AN7="Ja",IF(AK7="Ja",AL7,AL7-AH7),IF(AK7="Ja",AH7-R7,IF(U7="Ja",R7,"-")))</f>
@@ -1384,11 +1384,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="L4:U4"/>
-    <mergeCell ref="R5:U5"/>
     <mergeCell ref="W5:Y5"/>
     <mergeCell ref="Z5:AB5"/>
     <mergeCell ref="AP5:AW5"/>
@@ -1402,6 +1397,11 @@
     <mergeCell ref="AH4:AK5"/>
     <mergeCell ref="AL4:AN5"/>
     <mergeCell ref="AO4:AO6"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="L4:U4"/>
+    <mergeCell ref="R5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1606,18 +1606,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1640,6 +1640,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A18E2A5-8E58-4041-8327-21E9E81899ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5629F10-0798-4A91-8A47-B660EE7C0BA9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1654,12 +1662,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A18E2A5-8E58-4041-8327-21E9E81899ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
direct-to-dev: Change cell format in excel template
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu2\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B449DFFE-A155-4F4C-B4D0-AFB9113496EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CE32AC-EF82-4E3A-AA03-4F5CA664BC2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -524,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -566,6 +566,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -575,12 +581,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -605,14 +605,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -952,7 +956,9 @@
     <col min="23" max="24" width="22.7109375" customWidth="1"/>
     <col min="25" max="25" width="16.7109375" customWidth="1"/>
     <col min="26" max="27" width="22.85546875" customWidth="1"/>
-    <col min="28" max="42" width="16.7109375" customWidth="1"/>
+    <col min="28" max="40" width="16.7109375" customWidth="1"/>
+    <col min="41" max="41" width="16.7109375" style="34" customWidth="1"/>
+    <col min="42" max="42" width="16.7109375" customWidth="1"/>
     <col min="43" max="43" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="44" max="50" width="16.7109375" customWidth="1"/>
   </cols>
@@ -978,34 +984,34 @@
       <c r="B4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="23"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="25"/>
       <c r="V4" s="16"/>
-      <c r="W4" s="21" t="s">
+      <c r="W4" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="21" t="s">
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="23"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="24"/>
+      <c r="AG4" s="25"/>
       <c r="AH4" s="28" t="s">
         <v>18</v>
       </c>
@@ -1017,7 +1023,7 @@
       </c>
       <c r="AM4" s="29"/>
       <c r="AN4" s="30"/>
-      <c r="AO4" s="34" t="s">
+      <c r="AO4" s="35" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1079,17 +1085,17 @@
       <c r="AL5" s="31"/>
       <c r="AM5" s="32"/>
       <c r="AN5" s="33"/>
-      <c r="AO5" s="35"/>
-      <c r="AP5" s="24" t="s">
+      <c r="AO5" s="36"/>
+      <c r="AP5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AQ5" s="24"/>
-      <c r="AR5" s="24"/>
-      <c r="AS5" s="24"/>
-      <c r="AT5" s="24"/>
-      <c r="AU5" s="24"/>
-      <c r="AV5" s="24"/>
-      <c r="AW5" s="25"/>
+      <c r="AQ5" s="21"/>
+      <c r="AR5" s="21"/>
+      <c r="AS5" s="21"/>
+      <c r="AT5" s="21"/>
+      <c r="AU5" s="21"/>
+      <c r="AV5" s="21"/>
+      <c r="AW5" s="22"/>
     </row>
     <row r="6" spans="1:50" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1202,7 +1208,7 @@
       <c r="AN6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AO6" s="36"/>
+      <c r="AO6" s="37"/>
       <c r="AP6" s="19" t="s">
         <v>90</v>
       </c>
@@ -1349,7 +1355,7 @@
       <c r="AN7" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="AO7" s="17" t="str">
+      <c r="AO7" s="38" t="str">
         <f>IF(NOT(ISNUMBER(AL7)),AH7,AL7)</f>
         <v>{stufe2VerfuegungBetrag}</v>
       </c>
@@ -1384,6 +1390,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="L4:U4"/>
+    <mergeCell ref="R5:U5"/>
     <mergeCell ref="W5:Y5"/>
     <mergeCell ref="Z5:AB5"/>
     <mergeCell ref="AP5:AW5"/>
@@ -1397,11 +1408,6 @@
     <mergeCell ref="AH4:AK5"/>
     <mergeCell ref="AL4:AN5"/>
     <mergeCell ref="AO4:AO6"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="L4:U4"/>
-    <mergeCell ref="R5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1409,6 +1415,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100711209C60F5007419C092DB1F82A4795" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ddb10cc1903f988a2bdc77454b9dc4c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d53bc33c-7e51-42d1-8a72-72bcbf7ea968" xmlns:ns3="55df0d9a-b115-40a4-96c1-9261dc1f94e8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c657c3bfd70ec264372646d204a4f2b" ns2:_="" ns3:_="">
     <xsd:import namespace="d53bc33c-7e51-42d1-8a72-72bcbf7ea968"/>
@@ -1605,22 +1626,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5629F10-0798-4A91-8A47-B660EE7C0BA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="55df0d9a-b115-40a4-96c1-9261dc1f94e8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d53bc33c-7e51-42d1-8a72-72bcbf7ea968"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A18E2A5-8E58-4041-8327-21E9E81899ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA59B390-4D54-40A4-8874-4D75877374A7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1637,29 +1668,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A18E2A5-8E58-4041-8327-21E9E81899ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5629F10-0798-4A91-8A47-B660EE7C0BA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="55df0d9a-b115-40a4-96c1-9261dc1f94e8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d53bc33c-7e51-42d1-8a72-72bcbf7ea968"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
direct-to-dev Notrecht Excel Format Änderung
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Notrecht.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu2\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CE32AC-EF82-4E3A-AA03-4F5CA664BC2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AB95F4-B4CD-4127-B63A-D2CF6EF4F397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6295F66A-BE02-46FD-82C6-EF4FA7651A4F}"/>
   </bookViews>
@@ -605,18 +605,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -957,7 +959,7 @@
     <col min="25" max="25" width="16.7109375" customWidth="1"/>
     <col min="26" max="27" width="22.85546875" customWidth="1"/>
     <col min="28" max="40" width="16.7109375" customWidth="1"/>
-    <col min="41" max="41" width="16.7109375" style="34" customWidth="1"/>
+    <col min="41" max="41" width="16.7109375" style="37" customWidth="1"/>
     <col min="42" max="42" width="16.7109375" customWidth="1"/>
     <col min="43" max="43" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="44" max="50" width="16.7109375" customWidth="1"/>
@@ -1023,7 +1025,7 @@
       </c>
       <c r="AM4" s="29"/>
       <c r="AN4" s="30"/>
-      <c r="AO4" s="35" t="s">
+      <c r="AO4" s="34" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1085,7 +1087,7 @@
       <c r="AL5" s="31"/>
       <c r="AM5" s="32"/>
       <c r="AN5" s="33"/>
-      <c r="AO5" s="36"/>
+      <c r="AO5" s="35"/>
       <c r="AP5" s="21" t="s">
         <v>19</v>
       </c>
@@ -1208,7 +1210,7 @@
       <c r="AN6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AO6" s="37"/>
+      <c r="AO6" s="36"/>
       <c r="AP6" s="19" t="s">
         <v>90</v>
       </c>

</xml_diff>